<commit_message>
AA - budget_economico trasnformed to long
</commit_message>
<xml_diff>
--- a/inputs_mod/support_trascodifiche.xlsx
+++ b/inputs_mod/support_trascodifiche.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://innovationteam-my.sharepoint.com/personal/a_abraham_innovationteam_eu/Documents/Documenti/progetti/22p11_Tool_FA/inputs_mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{54BC2D7E-0A9F-44CA-9791-8F1FA2B4139E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{716D20F5-6C92-4157-8AB1-FD9D1C97BAA2}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="13_ncr:1_{54BC2D7E-0A9F-44CA-9791-8F1FA2B4139E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7A6516E-245B-4802-88C3-9D998F28AB32}"/>
   <bookViews>
-    <workbookView xWindow="1778" yWindow="1778" windowWidth="21600" windowHeight="11332" activeTab="1" xr2:uid="{9758A490-5BBA-4DAE-A128-35FF12EB83CB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" firstSheet="1" activeTab="4" xr2:uid="{9758A490-5BBA-4DAE-A128-35FF12EB83CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Condizioni_Commerciali" sheetId="7" r:id="rId1"/>
@@ -2472,6 +2472,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -6832,7 +6833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1868E1ED-CAEF-4CF4-8725-DD393E3F7908}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -7734,8 +7735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F3E4911-66FD-46BA-85EE-7208A8CAC824}">
   <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F113" sqref="F113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8680,7 +8681,7 @@
         <v>83</v>
       </c>
       <c r="E51" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.45">
@@ -9082,7 +9083,7 @@
         <v>83</v>
       </c>
       <c r="E73" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.45">
@@ -9136,7 +9137,7 @@
         <v>83</v>
       </c>
       <c r="E76" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.45">
@@ -9460,7 +9461,7 @@
         <v>83</v>
       </c>
       <c r="E94" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.45">

</xml_diff>